<commit_message>
Añadidos 2 botons a V_Principal
</commit_message>
<xml_diff>
--- a/ventas/pagos.xlsx
+++ b/ventas/pagos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
   <si>
     <t>IdPago</t>
   </si>
@@ -35,7 +35,7 @@
     <t>DiagnósticoBot</t>
   </si>
   <si>
-    <t>02/12/2025</t>
+    <t>03/12/2025</t>
   </si>
 </sst>
 </file>
@@ -80,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,13 +117,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>3750.0</v>
+        <v>2080.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>112.5</v>
+        <v>62.4</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>3637.5</v>
+        <v>2017.6</v>
       </c>
     </row>
     <row r="3">
@@ -134,13 +134,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>2080.0</v>
+        <v>80.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>62.4</v>
+        <v>2.4</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>2017.6</v>
+        <v>77.6</v>
       </c>
     </row>
     <row r="4">
@@ -151,13 +151,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>200.0</v>
+        <v>2600.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>6.0</v>
+        <v>78.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>194.0</v>
+        <v>2522.0</v>
       </c>
     </row>
     <row r="5">
@@ -168,13 +168,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>890.0</v>
+        <v>250.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>26.7</v>
+        <v>7.5</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>863.3</v>
+        <v>242.5</v>
       </c>
     </row>
     <row r="6">
@@ -185,13 +185,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>320.0</v>
+        <v>200.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>9.6</v>
+        <v>6.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>310.4</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="7">
@@ -202,13 +202,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>3000.0</v>
+        <v>2080.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>90.0</v>
+        <v>62.4</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>2910.0</v>
+        <v>2017.6</v>
       </c>
     </row>
     <row r="8">
@@ -219,13 +219,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>2800.0</v>
+        <v>400.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>84.0</v>
+        <v>12.0</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>2716.0</v>
+        <v>388.0</v>
       </c>
     </row>
     <row r="9">
@@ -236,13 +236,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>12500.0</v>
+        <v>200.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>375.0</v>
+        <v>6.0</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>12125.0</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="10">
@@ -253,13 +253,319 @@
         <v>7</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>650.0</v>
+        <v>160.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>19.5</v>
+        <v>4.8</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>630.5</v>
+        <v>155.2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>1.8293E7</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>2250.0</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>67.5</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>2182.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>1.8293001E7</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>240.0</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>7.199999999999999</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>232.8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>1.8293002E7</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>240.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>7.199999999999999</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>232.8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="0">
+        <v>1.8293003E7</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C14" t="n" s="0">
+        <v>3000.0</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>90.0</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>2910.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="0">
+        <v>1.8293004E7</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>2670.0</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>80.1</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>2589.9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n" s="0">
+        <v>1.8293005E7</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>750.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>22.5</v>
+      </c>
+      <c r="E16" t="n" s="0">
+        <v>727.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="0">
+        <v>1.8293006E7</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="E17" t="n" s="0">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="0">
+        <v>1.8293007E7</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C18" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="D18" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="E18" t="n" s="0">
+        <v>194.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="0">
+        <v>1.8293008E7</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C19" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="E19" t="n" s="0">
+        <v>388.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="0">
+        <v>1.8293E7</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C20" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="E20" t="n" s="0">
+        <v>194.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>1.8293001E7</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C21" t="n" s="0">
+        <v>250.0</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="E21" t="n" s="0">
+        <v>242.5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>1.8293002E7</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>2250.0</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>67.5</v>
+      </c>
+      <c r="E22" t="n" s="0">
+        <v>2182.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>1.8293003E7</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>3000.0</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>90.0</v>
+      </c>
+      <c r="E23" t="n" s="0">
+        <v>2910.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="0">
+        <v>1.8293004E7</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C24" t="n" s="0">
+        <v>2670.0</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>80.1</v>
+      </c>
+      <c r="E24" t="n" s="0">
+        <v>2589.9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n" s="0">
+        <v>1.8293005E7</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C25" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="D25" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="E25" t="n" s="0">
+        <v>194.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="0">
+        <v>1.8293006E7</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C26" t="n" s="0">
+        <v>80.0</v>
+      </c>
+      <c r="D26" t="n" s="0">
+        <v>2.4</v>
+      </c>
+      <c r="E26" t="n" s="0">
+        <v>77.6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n" s="0">
+        <v>1.8293007E7</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C27" t="n" s="0">
+        <v>2250.0</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>67.5</v>
+      </c>
+      <c r="E27" t="n" s="0">
+        <v>2182.5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="0">
+        <v>1.8293008E7</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D28" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E28" t="n" s="0">
+        <v>97.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejorada  la funcionalidad para generar ventas en la persistencia
</commit_message>
<xml_diff>
--- a/ventas/pagos.xlsx
+++ b/ventas/pagos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
   <si>
     <t>IdPago</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,13 +117,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>2080.0</v>
+        <v>1560.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>62.4</v>
+        <v>46.8</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>2017.6</v>
+        <v>1513.2</v>
       </c>
     </row>
     <row r="3">
@@ -134,13 +134,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>80.0</v>
+        <v>890.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>2.4</v>
+        <v>26.7</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>77.6</v>
+        <v>863.3</v>
       </c>
     </row>
     <row r="4">
@@ -151,13 +151,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>2600.0</v>
+        <v>1780.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>78.0</v>
+        <v>53.4</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>2522.0</v>
+        <v>1726.6</v>
       </c>
     </row>
     <row r="5">
@@ -168,13 +168,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>250.0</v>
+        <v>160.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>7.5</v>
+        <v>4.8</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>242.5</v>
+        <v>155.2</v>
       </c>
     </row>
     <row r="6">
@@ -185,13 +185,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>200.0</v>
+        <v>240.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>6.0</v>
+        <v>7.199999999999999</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>194.0</v>
+        <v>232.8</v>
       </c>
     </row>
     <row r="7">
@@ -202,13 +202,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>2080.0</v>
+        <v>150.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>62.4</v>
+        <v>4.5</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>2017.6</v>
+        <v>145.5</v>
       </c>
     </row>
     <row r="8">
@@ -219,13 +219,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>400.0</v>
+        <v>890.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>12.0</v>
+        <v>26.7</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>388.0</v>
+        <v>863.3</v>
       </c>
     </row>
     <row r="9">
@@ -236,13 +236,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>200.0</v>
+        <v>2080.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>6.0</v>
+        <v>62.4</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>194.0</v>
+        <v>2017.6</v>
       </c>
     </row>
     <row r="10">
@@ -253,13 +253,13 @@
         <v>7</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>160.0</v>
+        <v>100.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>4.8</v>
+        <v>3.0</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>155.2</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="11">
@@ -270,13 +270,13 @@
         <v>7</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>2250.0</v>
+        <v>200.0</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>67.5</v>
+        <v>6.0</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>2182.5</v>
+        <v>194.0</v>
       </c>
     </row>
     <row r="12">
@@ -287,13 +287,13 @@
         <v>7</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>240.0</v>
+        <v>100.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>7.199999999999999</v>
+        <v>3.0</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>232.8</v>
+        <v>97.0</v>
       </c>
     </row>
     <row r="13">
@@ -304,13 +304,13 @@
         <v>7</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>240.0</v>
+        <v>1780.0</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>7.199999999999999</v>
+        <v>53.4</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>232.8</v>
+        <v>1726.6</v>
       </c>
     </row>
     <row r="14">
@@ -321,13 +321,13 @@
         <v>7</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>3000.0</v>
+        <v>2250.0</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>90.0</v>
+        <v>67.5</v>
       </c>
       <c r="E14" t="n" s="0">
-        <v>2910.0</v>
+        <v>2182.5</v>
       </c>
     </row>
     <row r="15">
@@ -338,13 +338,13 @@
         <v>7</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>2670.0</v>
+        <v>4450.0</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>80.1</v>
+        <v>133.5</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>2589.9</v>
+        <v>4316.5</v>
       </c>
     </row>
     <row r="16">
@@ -355,13 +355,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>750.0</v>
+        <v>1040.0</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>22.5</v>
+        <v>31.2</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>727.5</v>
+        <v>1008.8</v>
       </c>
     </row>
     <row r="17">
@@ -372,13 +372,13 @@
         <v>7</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>50.0</v>
+        <v>320.0</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>1.5</v>
+        <v>9.6</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>48.5</v>
+        <v>310.4</v>
       </c>
     </row>
     <row r="18">
@@ -389,13 +389,13 @@
         <v>7</v>
       </c>
       <c r="C18" t="n" s="0">
-        <v>200.0</v>
+        <v>3560.0</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>6.0</v>
+        <v>106.8</v>
       </c>
       <c r="E18" t="n" s="0">
-        <v>194.0</v>
+        <v>3453.2</v>
       </c>
     </row>
     <row r="19">
@@ -406,166 +406,13 @@
         <v>7</v>
       </c>
       <c r="C19" t="n" s="0">
-        <v>400.0</v>
+        <v>240.0</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>12.0</v>
+        <v>7.199999999999999</v>
       </c>
       <c r="E19" t="n" s="0">
-        <v>388.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n" s="0">
-        <v>1.8293E7</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C20" t="n" s="0">
-        <v>200.0</v>
-      </c>
-      <c r="D20" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="E20" t="n" s="0">
-        <v>194.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n" s="0">
-        <v>1.8293001E7</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C21" t="n" s="0">
-        <v>250.0</v>
-      </c>
-      <c r="D21" t="n" s="0">
-        <v>7.5</v>
-      </c>
-      <c r="E21" t="n" s="0">
-        <v>242.5</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n" s="0">
-        <v>1.8293002E7</v>
-      </c>
-      <c r="B22" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C22" t="n" s="0">
-        <v>2250.0</v>
-      </c>
-      <c r="D22" t="n" s="0">
-        <v>67.5</v>
-      </c>
-      <c r="E22" t="n" s="0">
-        <v>2182.5</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n" s="0">
-        <v>1.8293003E7</v>
-      </c>
-      <c r="B23" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C23" t="n" s="0">
-        <v>3000.0</v>
-      </c>
-      <c r="D23" t="n" s="0">
-        <v>90.0</v>
-      </c>
-      <c r="E23" t="n" s="0">
-        <v>2910.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n" s="0">
-        <v>1.8293004E7</v>
-      </c>
-      <c r="B24" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C24" t="n" s="0">
-        <v>2670.0</v>
-      </c>
-      <c r="D24" t="n" s="0">
-        <v>80.1</v>
-      </c>
-      <c r="E24" t="n" s="0">
-        <v>2589.9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n" s="0">
-        <v>1.8293005E7</v>
-      </c>
-      <c r="B25" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C25" t="n" s="0">
-        <v>200.0</v>
-      </c>
-      <c r="D25" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="E25" t="n" s="0">
-        <v>194.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n" s="0">
-        <v>1.8293006E7</v>
-      </c>
-      <c r="B26" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C26" t="n" s="0">
-        <v>80.0</v>
-      </c>
-      <c r="D26" t="n" s="0">
-        <v>2.4</v>
-      </c>
-      <c r="E26" t="n" s="0">
-        <v>77.6</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n" s="0">
-        <v>1.8293007E7</v>
-      </c>
-      <c r="B27" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C27" t="n" s="0">
-        <v>2250.0</v>
-      </c>
-      <c r="D27" t="n" s="0">
-        <v>67.5</v>
-      </c>
-      <c r="E27" t="n" s="0">
-        <v>2182.5</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n" s="0">
-        <v>1.8293008E7</v>
-      </c>
-      <c r="B28" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C28" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="D28" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="E28" t="n" s="0">
-        <v>97.0</v>
+        <v>232.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no se que hice
</commit_message>
<xml_diff>
--- a/ventas/pagos.xlsx
+++ b/ventas/pagos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>IdPago</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,13 +117,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>1560.0</v>
+        <v>80.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>46.8</v>
+        <v>2.4</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>1513.2</v>
+        <v>77.6</v>
       </c>
     </row>
     <row r="3">
@@ -134,13 +134,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>890.0</v>
+        <v>320.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>26.7</v>
+        <v>9.6</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>863.3</v>
+        <v>310.4</v>
       </c>
     </row>
     <row r="4">
@@ -151,13 +151,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>1780.0</v>
+        <v>80.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>53.4</v>
+        <v>2.4</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>1726.6</v>
+        <v>77.6</v>
       </c>
     </row>
     <row r="5">
@@ -168,13 +168,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>160.0</v>
+        <v>150.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>155.2</v>
+        <v>145.5</v>
       </c>
     </row>
     <row r="6">
@@ -185,13 +185,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>240.0</v>
+        <v>3560.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>7.199999999999999</v>
+        <v>106.8</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>232.8</v>
+        <v>3453.2</v>
       </c>
     </row>
     <row r="7">
@@ -202,13 +202,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>150.0</v>
+        <v>2670.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>4.5</v>
+        <v>80.1</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>145.5</v>
+        <v>2589.9</v>
       </c>
     </row>
     <row r="8">
@@ -219,13 +219,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>890.0</v>
+        <v>1500.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>26.7</v>
+        <v>45.0</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>863.3</v>
+        <v>1455.0</v>
       </c>
     </row>
     <row r="9">
@@ -236,13 +236,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>2080.0</v>
+        <v>80.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>62.4</v>
+        <v>2.4</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>2017.6</v>
+        <v>77.6</v>
       </c>
     </row>
     <row r="10">
@@ -253,166 +253,13 @@
         <v>7</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>3.0</v>
+        <v>2.4</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>97.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n" s="0">
-        <v>1.8293E7</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C11" t="n" s="0">
-        <v>200.0</v>
-      </c>
-      <c r="D11" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="E11" t="n" s="0">
-        <v>194.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n" s="0">
-        <v>1.8293001E7</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C12" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="D12" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="E12" t="n" s="0">
-        <v>97.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n" s="0">
-        <v>1.8293002E7</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C13" t="n" s="0">
-        <v>1780.0</v>
-      </c>
-      <c r="D13" t="n" s="0">
-        <v>53.4</v>
-      </c>
-      <c r="E13" t="n" s="0">
-        <v>1726.6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n" s="0">
-        <v>1.8293003E7</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C14" t="n" s="0">
-        <v>2250.0</v>
-      </c>
-      <c r="D14" t="n" s="0">
-        <v>67.5</v>
-      </c>
-      <c r="E14" t="n" s="0">
-        <v>2182.5</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n" s="0">
-        <v>1.8293004E7</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C15" t="n" s="0">
-        <v>4450.0</v>
-      </c>
-      <c r="D15" t="n" s="0">
-        <v>133.5</v>
-      </c>
-      <c r="E15" t="n" s="0">
-        <v>4316.5</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n" s="0">
-        <v>1.8293005E7</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C16" t="n" s="0">
-        <v>1040.0</v>
-      </c>
-      <c r="D16" t="n" s="0">
-        <v>31.2</v>
-      </c>
-      <c r="E16" t="n" s="0">
-        <v>1008.8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n" s="0">
-        <v>1.8293006E7</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C17" t="n" s="0">
-        <v>320.0</v>
-      </c>
-      <c r="D17" t="n" s="0">
-        <v>9.6</v>
-      </c>
-      <c r="E17" t="n" s="0">
-        <v>310.4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n" s="0">
-        <v>1.8293007E7</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C18" t="n" s="0">
-        <v>3560.0</v>
-      </c>
-      <c r="D18" t="n" s="0">
-        <v>106.8</v>
-      </c>
-      <c r="E18" t="n" s="0">
-        <v>3453.2</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n" s="0">
-        <v>1.8293008E7</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C19" t="n" s="0">
-        <v>240.0</v>
-      </c>
-      <c r="D19" t="n" s="0">
-        <v>7.199999999999999</v>
-      </c>
-      <c r="E19" t="n" s="0">
-        <v>232.8</v>
+        <v>77.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>